<commit_message>
various chnages in implementing reframe
</commit_message>
<xml_diff>
--- a/REFramework_BlaackBook/Blackbook.xlsx
+++ b/REFramework_BlaackBook/Blackbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/mshanmug_stevens_edu/Documents/Documents/UiPath/Blackbook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive - stevens.edu\Documents\GitHub\Automation-Projects\REFramework_BlaackBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{0BC5ADF3-863D-4909-B691-2322F6420CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAD56DF8-9274-4EFC-AD5F-652045189D3F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8D0E76-8A14-45D6-B8FC-DA86DD4FC0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4728" yWindow="3636" windowWidth="9636" windowHeight="6564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1296" yWindow="1152" windowWidth="14400" windowHeight="7344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fruit</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Banana</t>
-  </si>
-  <si>
-    <t>Apple and pineapple tray cake</t>
   </si>
   <si>
     <t>Cauliflower, fennel and orange salad</t>
@@ -398,11 +395,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -410,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -421,7 +415,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -429,10 +423,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5">
         <v>7</v>

</xml_diff>

<commit_message>
Final major changes done during developing
</commit_message>
<xml_diff>
--- a/REFramework_BlaackBook/Blackbook.xlsx
+++ b/REFramework_BlaackBook/Blackbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive - stevens.edu\Documents\GitHub\Automation-Projects\REFramework_BlaackBook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/mshanmug_stevens_edu/Documents/Documents/GitHub/Automation-Projects/REFramework_BlaackBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8D0E76-8A14-45D6-B8FC-DA86DD4FC0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{7B8D0E76-8A14-45D6-B8FC-DA86DD4FC0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D35D054-3E74-4762-8977-F93A6539AAA3}"/>
   <bookViews>
     <workbookView xWindow="1296" yWindow="1152" windowWidth="14400" windowHeight="7344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Fruit</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>Vodka, guava and ginger cocktail</t>
+  </si>
+  <si>
+    <t>papaya</t>
+  </si>
+  <si>
+    <t>Salmon tacos with papaya salsa</t>
+  </si>
+  <si>
+    <t>passion fruit</t>
+  </si>
+  <si>
+    <t>Glen of passion</t>
+  </si>
+  <si>
+    <t>plum</t>
+  </si>
+  <si>
+    <t>Mini plum crostatas</t>
+  </si>
+  <si>
+    <t>Apple and cinnamon choux fritters</t>
   </si>
 </sst>
 </file>
@@ -372,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -395,8 +416,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
       <c r="C2">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -430,6 +454,39 @@
       </c>
       <c r="C5">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>